<commit_message>
[R volatility options] added gridsearc +parameter results in R-file
</commit_message>
<xml_diff>
--- a/R/r_output/table_1_mat.xlsx
+++ b/R/r_output/table_1_mat.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">current_day_estimation</t>
   </si>
@@ -26,10 +26,103 @@
     <t xml:space="preserve">sigma</t>
   </si>
   <si>
+    <t xml:space="preserve">Min_of_Loss_Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">convergence_code</t>
+  </si>
+  <si>
     <t xml:space="preserve">number_options</t>
   </si>
   <si>
     <t xml:space="preserve">future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42.8763013530862</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.6098720539757</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.775679522497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.69523976311823</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45.3357355953877</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.3196151477721</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23.1406231715724</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.19183864895222</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.2616518161135</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.0501361318493</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.5027277643546</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.49889322333684</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55.4283633869522</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33.7547600930658</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29.2313237429204</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.46244060702908</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56.6554010930514</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.6599768985326</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28.1071616282124</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.9518800745399</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66.7167033510985</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43.6430444924148</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37.226956067394</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.48874584633205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59.7786538985285</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44.886193000946</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38.5993295660477</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.3485341677696</t>
   </si>
 </sst>
 </file>
@@ -386,24 +479,36 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
         <v>43895</v>
       </c>
-      <c r="B2" t="n">
-        <v>42.8555487708366</v>
-      </c>
-      <c r="C2" t="n">
-        <v>23.6096591372216</v>
-      </c>
-      <c r="D2" t="n">
-        <v>18.7710511020664</v>
-      </c>
-      <c r="E2" t="n">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="n">
         <v>23</v>
       </c>
-      <c r="F2" t="n">
+      <c r="H2" t="n">
         <v>1</v>
       </c>
     </row>
@@ -411,19 +516,25 @@
       <c r="A3" s="1" t="n">
         <v>43896</v>
       </c>
-      <c r="B3" t="n">
-        <v>45.3337089018745</v>
-      </c>
-      <c r="C3" t="n">
-        <v>29.319591672174</v>
-      </c>
-      <c r="D3" t="n">
-        <v>23.140092519293</v>
-      </c>
-      <c r="E3" t="n">
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="n">
         <v>27</v>
       </c>
-      <c r="F3" t="n">
+      <c r="H3" t="n">
         <v>1</v>
       </c>
     </row>
@@ -431,19 +542,25 @@
       <c r="A4" s="1" t="n">
         <v>43899</v>
       </c>
-      <c r="B4" t="n">
-        <v>60.1272281303963</v>
-      </c>
-      <c r="C4" t="n">
-        <v>33.0287380469169</v>
-      </c>
-      <c r="D4" t="n">
-        <v>33.1077978786204</v>
-      </c>
-      <c r="E4" t="n">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="n">
         <v>32</v>
       </c>
-      <c r="F4" t="n">
+      <c r="H4" t="n">
         <v>1</v>
       </c>
     </row>
@@ -451,19 +568,25 @@
       <c r="A5" s="1" t="n">
         <v>43900</v>
       </c>
-      <c r="B5" t="n">
-        <v>55.4191953211351</v>
-      </c>
-      <c r="C5" t="n">
-        <v>33.7546736696786</v>
-      </c>
-      <c r="D5" t="n">
-        <v>29.2288635282043</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="n">
         <v>32</v>
       </c>
-      <c r="F5" t="n">
+      <c r="H5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -471,19 +594,25 @@
       <c r="A6" s="1" t="n">
         <v>43901</v>
       </c>
-      <c r="B6" t="n">
-        <v>56.6408845510411</v>
-      </c>
-      <c r="C6" t="n">
-        <v>34.6598335295871</v>
-      </c>
-      <c r="D6" t="n">
-        <v>28.1035220620328</v>
-      </c>
-      <c r="E6" t="n">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
         <v>28</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="n">
+        <v>28</v>
+      </c>
+      <c r="H6" t="n">
         <v>1</v>
       </c>
     </row>
@@ -491,19 +620,25 @@
       <c r="A7" s="1" t="n">
         <v>43902</v>
       </c>
-      <c r="B7" t="n">
-        <v>66.4610541240932</v>
-      </c>
-      <c r="C7" t="n">
-        <v>43.641255390251</v>
-      </c>
-      <c r="D7" t="n">
-        <v>37.154931314669</v>
-      </c>
-      <c r="E7" t="n">
+      <c r="B7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="n">
         <v>25</v>
       </c>
-      <c r="F7" t="n">
+      <c r="H7" t="n">
         <v>1</v>
       </c>
     </row>
@@ -511,19 +646,25 @@
       <c r="A8" s="1" t="n">
         <v>43903</v>
       </c>
-      <c r="B8" t="n">
-        <v>59.7759425772485</v>
-      </c>
-      <c r="C8" t="n">
-        <v>44.8861549725936</v>
-      </c>
-      <c r="D8" t="n">
-        <v>38.5984132887144</v>
-      </c>
-      <c r="E8" t="n">
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
         <v>30</v>
       </c>
-      <c r="F8" t="n">
+      <c r="H8" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>